<commit_message>
Correct harmo rule containing rowMeans
</commit_message>
<xml_diff>
--- a/data_processing_elements-NHS.xlsx
+++ b/data_processing_elements-NHS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134F38FF-0F81-42CC-ADE0-392EDD7B5986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EA4BCA-9431-4EBE-9081-F31DD6287889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_processing_elements!$A$1:$U$84</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1403,12 +1403,6 @@
     <t>ifelse(!is.na(BIAPbf_NT4BLM), "Bioelectrical impedance measurement (InBody 770)", NA)</t>
   </si>
   <si>
-    <t>round(rowMeans(select(., BPSyst1_NT4BLM, BPSyst2_NT4BLM, BPSyst3_NT4BLM), na.rm=TRUE), 2)</t>
-  </si>
-  <si>
-    <t>round(rowMeans(select(., BPDias1_NT4BLM, BPDias2_NT4BLM, BPDias3_NT4BLM), na.rm=TRUE), 2)</t>
-  </si>
-  <si>
     <t>round(SeChol_NT4BLM - SeHDLChol_NT4BLM - (SeTrig_NT4BLM/2.2), 2)</t>
   </si>
   <si>
@@ -1614,6 +1608,14 @@
   <si>
     <t>Please provide ID variable
 Is it really the id variable name ?</t>
+  </si>
+  <si>
+    <t>case_when(is.na(BPSyst1_NT4BLM) &amp; is.na(BPSyst2_NT4BLM) &amp; is.na(BPSyst3_NT4BLM) ~ NA;
+ELSE ~ round(rowMeans(select(., BPSyst1_NT4BLM, BPSyst2_NT4BLM, BPSyst3_NT4BLM), na.rm=TRUE), 2))</t>
+  </si>
+  <si>
+    <t>case_when(is.na(BPDias1_NT4BLM) &amp; is.na(BPDias2_NT4BLM) &amp; is.na(BPDias3_NT4BLM) ~ NA;
+ELSE ~ round(rowMeans(select(., BPDias1_NT4BLM, BPDias2_NT4BLM, BPDias3_NT4BLM), na.rm=TRUE), 2))</t>
   </si>
 </sst>
 </file>
@@ -1752,7 +1754,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1774,7 +1776,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2096,10 +2098,10 @@
       <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R11" sqref="R11"/>
+      <selection pane="bottomRight" activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="13" customWidth="1"/>
@@ -2119,7 +2121,7 @@
     <col min="16" max="16" width="12.7109375" style="13" customWidth="1"/>
     <col min="17" max="17" width="12.42578125" style="13" customWidth="1"/>
     <col min="18" max="18" width="17.5703125" style="13" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" style="13" customWidth="1"/>
+    <col min="19" max="19" width="71.5703125" style="13" customWidth="1"/>
     <col min="20" max="20" width="25.5703125" style="13" customWidth="1"/>
     <col min="21" max="21" width="25.28515625" style="13" customWidth="1"/>
   </cols>
@@ -2227,7 +2229,7 @@
         <v>401</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="U2" s="1"/>
     </row>
@@ -2254,7 +2256,7 @@
         <v>31</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>296</v>
@@ -2275,7 +2277,7 @@
         <v>32</v>
       </c>
       <c r="S3" s="13" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
@@ -2342,10 +2344,10 @@
         <v>42</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>299</v>
@@ -2360,7 +2362,7 @@
         <v>32</v>
       </c>
       <c r="S5" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="U5" s="1"/>
     </row>
@@ -2387,7 +2389,7 @@
         <v>47</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="K6" s="13" t="s">
         <v>289</v>
@@ -2475,7 +2477,7 @@
         <v>57</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>302</v>
@@ -2520,7 +2522,7 @@
         <v>63</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>304</v>
@@ -2602,7 +2604,7 @@
         <v>24</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>307</v>
@@ -2623,7 +2625,7 @@
         <v>203</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="U11" s="1"/>
     </row>
@@ -2689,7 +2691,7 @@
         <v>78</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="K13" s="13" t="s">
         <v>290</v>
@@ -2776,7 +2778,7 @@
         <v>85</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="K15" s="13" t="s">
         <v>312</v>
@@ -2824,7 +2826,7 @@
         <v>88</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="K16" s="13" t="s">
         <v>291</v>
@@ -2866,7 +2868,7 @@
         <v>91</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="P17" s="13" t="s">
         <v>25</v>
@@ -2906,7 +2908,7 @@
         <v>94</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="K18" s="13" t="s">
         <v>294</v>
@@ -2948,7 +2950,7 @@
         <v>91</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="P19" s="13" t="s">
         <v>25</v>
@@ -2988,7 +2990,7 @@
         <v>99</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="K20" s="13" t="s">
         <v>313</v>
@@ -3030,7 +3032,7 @@
         <v>88</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K21" s="13" t="s">
         <v>314</v>
@@ -3072,7 +3074,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="P22" s="13" t="s">
         <v>25</v>
@@ -3112,7 +3114,7 @@
         <v>107</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>315</v>
@@ -3154,7 +3156,7 @@
         <v>24</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>315</v>
@@ -3176,7 +3178,7 @@
       </c>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="1:21" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>24</v>
       </c>
@@ -3199,7 +3201,7 @@
         <v>113</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="K25" s="10" t="s">
         <v>317</v>
@@ -3217,10 +3219,10 @@
         <v>48</v>
       </c>
       <c r="R25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>406</v>
+        <v>203</v>
+      </c>
+      <c r="S25" s="11" t="s">
+        <v>460</v>
       </c>
       <c r="U25" s="1"/>
     </row>
@@ -3247,7 +3249,7 @@
         <v>113</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K26" s="10" t="s">
         <v>319</v>
@@ -3265,10 +3267,10 @@
         <v>48</v>
       </c>
       <c r="R26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>407</v>
+        <v>203</v>
+      </c>
+      <c r="S26" s="11" t="s">
+        <v>461</v>
       </c>
       <c r="U26" s="1"/>
     </row>
@@ -3295,7 +3297,7 @@
         <v>119</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K27" s="13" t="s">
         <v>321</v>
@@ -3382,7 +3384,7 @@
         <v>125</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K29" s="13" t="s">
         <v>324</v>
@@ -3430,7 +3432,7 @@
         <v>128</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K30" s="13" t="s">
         <v>328</v>
@@ -3478,7 +3480,7 @@
         <v>131</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>330</v>
@@ -3526,7 +3528,7 @@
         <v>134</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="K32" s="13" t="s">
         <v>331</v>
@@ -3574,7 +3576,7 @@
         <v>134</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>333</v>
@@ -3661,7 +3663,7 @@
         <v>134</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="K35" s="11" t="s">
         <v>335</v>
@@ -3682,7 +3684,7 @@
         <v>32</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="U35" s="1"/>
     </row>
@@ -3709,7 +3711,7 @@
         <v>134</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K36" s="13" t="s">
         <v>337</v>
@@ -3757,7 +3759,7 @@
         <v>145</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K37" s="13" t="s">
         <v>339</v>
@@ -3844,7 +3846,7 @@
         <v>155</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="K39" s="13" t="s">
         <v>341</v>
@@ -3934,7 +3936,7 @@
         <v>155</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="K41" s="13" t="s">
         <v>346</v>
@@ -4024,7 +4026,7 @@
         <v>168</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="K43" s="13" t="s">
         <v>348</v>
@@ -4072,7 +4074,7 @@
         <v>171</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="K44" s="13" t="s">
         <v>350</v>
@@ -4123,7 +4125,7 @@
         <v>175</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="K45" s="13" t="s">
         <v>174</v>
@@ -4173,7 +4175,7 @@
         <v>178</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="K46" s="13" t="s">
         <v>174</v>
@@ -4222,7 +4224,7 @@
         <v>181</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K47" s="13" t="s">
         <v>357</v>
@@ -4246,7 +4248,7 @@
         <v>32</v>
       </c>
       <c r="S47" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="U47" s="1"/>
     </row>
@@ -4273,7 +4275,7 @@
         <v>184</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="K48" s="13" t="s">
         <v>361</v>
@@ -4321,7 +4323,7 @@
         <v>188</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="K49" s="10" t="s">
         <v>364</v>
@@ -4345,7 +4347,7 @@
         <v>203</v>
       </c>
       <c r="S49" s="10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="U49" s="1"/>
     </row>
@@ -4372,7 +4374,7 @@
         <v>188</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="K50" s="10" t="s">
         <v>368</v>
@@ -4396,7 +4398,7 @@
         <v>203</v>
       </c>
       <c r="S50" s="10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="U50" s="1"/>
     </row>
@@ -4423,7 +4425,7 @@
         <v>188</v>
       </c>
       <c r="J51" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="K51" s="13" t="s">
         <v>371</v>
@@ -4510,7 +4512,7 @@
         <v>188</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="K53" s="13" t="s">
         <v>373</v>
@@ -4597,7 +4599,7 @@
         <v>188</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>375</v>
@@ -4645,7 +4647,7 @@
         <v>188</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>377</v>
@@ -5062,7 +5064,7 @@
         <v>230</v>
       </c>
       <c r="J67" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="K67" s="13" t="s">
         <v>379</v>
@@ -5110,7 +5112,7 @@
         <v>233</v>
       </c>
       <c r="J68" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="K68" s="13" t="s">
         <v>379</v>
@@ -5128,7 +5130,7 @@
         <v>203</v>
       </c>
       <c r="S68" s="11" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="U68" s="1"/>
     </row>
@@ -5155,7 +5157,7 @@
         <v>236</v>
       </c>
       <c r="J69" s="13" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>382</v>
@@ -5203,7 +5205,7 @@
         <v>239</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>385</v>
@@ -5368,7 +5370,7 @@
         <v>251</v>
       </c>
       <c r="J74" s="13" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>389</v>
@@ -5455,7 +5457,7 @@
         <v>230</v>
       </c>
       <c r="J76" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="K76" s="13" t="s">
         <v>391</v>
@@ -5500,7 +5502,7 @@
         <v>262</v>
       </c>
       <c r="J77" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="K77" s="13" t="s">
         <v>391</v>
@@ -5515,7 +5517,7 @@
         <v>203</v>
       </c>
       <c r="S77" s="11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="U77" s="1"/>
     </row>
@@ -5620,7 +5622,7 @@
         <v>188</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K80" s="13" t="s">
         <v>393</v>

</xml_diff>

<commit_message>
Correct value type for vegetable and fruit
</commit_message>
<xml_diff>
--- a/data_processing_elements-NHS.xlsx
+++ b/data_processing_elements-NHS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EA4BCA-9431-4EBE-9081-F31DD6287889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E66CE4-4D35-4817-B88B-2B43258B617B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -988,9 +988,6 @@
     <t>HbA1c</t>
   </si>
   <si>
-    <t>4 times a week is considered as dayly/almost daily</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
@@ -1616,6 +1613,9 @@
   <si>
     <t>case_when(is.na(BPDias1_NT4BLM) &amp; is.na(BPDias2_NT4BLM) &amp; is.na(BPDias3_NT4BLM) ~ NA;
 ELSE ~ round(rowMeans(select(., BPDias1_NT4BLM, BPDias2_NT4BLM, BPDias3_NT4BLM), na.rm=TRUE), 2))</t>
+  </si>
+  <si>
+    <t>4 times a week or more is considered as dayly/almost daily</t>
   </si>
 </sst>
 </file>
@@ -2095,10 +2095,10 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S9" sqref="S9"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>21</v>
@@ -2211,10 +2211,10 @@
         <v>24</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P2" s="13" t="s">
         <v>25</v>
@@ -2223,13 +2223,13 @@
         <v>26</v>
       </c>
       <c r="R2" s="13" t="s">
+        <v>399</v>
+      </c>
+      <c r="S2" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="S2" s="13" t="s">
-        <v>401</v>
-      </c>
       <c r="T2" s="16" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="U2" s="1"/>
     </row>
@@ -2238,7 +2238,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>27</v>
@@ -2256,16 +2256,16 @@
         <v>31</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K3" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="N3" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>298</v>
       </c>
       <c r="P3" s="13" t="s">
         <v>25</v>
@@ -2277,7 +2277,7 @@
         <v>32</v>
       </c>
       <c r="S3" s="13" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
@@ -2287,7 +2287,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>33</v>
@@ -2326,7 +2326,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>39</v>
@@ -2344,13 +2344,13 @@
         <v>42</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P5" s="13" t="s">
         <v>25</v>
@@ -2362,7 +2362,7 @@
         <v>32</v>
       </c>
       <c r="S5" s="13" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="U5" s="1"/>
     </row>
@@ -2371,7 +2371,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>44</v>
@@ -2389,16 +2389,16 @@
         <v>47</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K6" s="13" t="s">
         <v>289</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="M6" s="9" t="s">
         <v>300</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>301</v>
       </c>
       <c r="P6" s="13" t="s">
         <v>25</v>
@@ -2410,7 +2410,7 @@
         <v>38</v>
       </c>
       <c r="S6" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -2420,7 +2420,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>49</v>
@@ -2459,7 +2459,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>54</v>
@@ -2477,13 +2477,13 @@
         <v>57</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K8" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="P8" s="13" t="s">
         <v>25</v>
@@ -2504,7 +2504,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>60</v>
@@ -2522,16 +2522,16 @@
         <v>63</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K9" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="O9" s="13" t="s">
         <v>305</v>
-      </c>
-      <c r="O9" s="13" t="s">
-        <v>306</v>
       </c>
       <c r="P9" s="13" t="s">
         <v>25</v>
@@ -2552,7 +2552,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>64</v>
@@ -2589,7 +2589,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>68</v>
@@ -2604,16 +2604,16 @@
         <v>24</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="9" t="s">
         <v>308</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>309</v>
       </c>
       <c r="P11" s="13" t="s">
         <v>25</v>
@@ -2625,7 +2625,7 @@
         <v>203</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="U11" s="1"/>
     </row>
@@ -2634,7 +2634,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>71</v>
@@ -2673,7 +2673,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>75</v>
@@ -2691,7 +2691,7 @@
         <v>78</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K13" s="13" t="s">
         <v>290</v>
@@ -2700,7 +2700,7 @@
         <v>290</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P13" s="13" t="s">
         <v>25</v>
@@ -2712,7 +2712,7 @@
         <v>38</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U13" s="1"/>
     </row>
@@ -2721,7 +2721,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>79</v>
@@ -2760,7 +2760,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>83</v>
@@ -2778,13 +2778,13 @@
         <v>85</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P15" s="13" t="s">
         <v>25</v>
@@ -2799,7 +2799,7 @@
         <v>43</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="U15" s="1"/>
     </row>
@@ -2808,7 +2808,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>86</v>
@@ -2826,7 +2826,7 @@
         <v>88</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K16" s="13" t="s">
         <v>291</v>
@@ -2850,7 +2850,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>89</v>
@@ -2868,7 +2868,7 @@
         <v>91</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="P17" s="13" t="s">
         <v>25</v>
@@ -2880,7 +2880,7 @@
         <v>32</v>
       </c>
       <c r="S17" s="13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
@@ -2890,7 +2890,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>92</v>
@@ -2908,10 +2908,10 @@
         <v>94</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P18" s="13" t="s">
         <v>25</v>
@@ -2932,7 +2932,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>95</v>
@@ -2950,7 +2950,7 @@
         <v>91</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P19" s="13" t="s">
         <v>25</v>
@@ -2962,7 +2962,7 @@
         <v>32</v>
       </c>
       <c r="S19" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -2972,7 +2972,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>97</v>
@@ -2990,10 +2990,10 @@
         <v>99</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P20" s="13" t="s">
         <v>25</v>
@@ -3014,7 +3014,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>100</v>
@@ -3032,10 +3032,10 @@
         <v>88</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P21" s="13" t="s">
         <v>25</v>
@@ -3056,7 +3056,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>103</v>
@@ -3074,7 +3074,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="P22" s="13" t="s">
         <v>25</v>
@@ -3086,7 +3086,7 @@
         <v>32</v>
       </c>
       <c r="S22" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -3096,7 +3096,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>105</v>
@@ -3114,13 +3114,13 @@
         <v>107</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K23" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="L23" s="13" t="s">
         <v>315</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>316</v>
       </c>
       <c r="P23" s="13" t="s">
         <v>25</v>
@@ -3141,7 +3141,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>108</v>
@@ -3156,13 +3156,13 @@
         <v>24</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K24" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="L24" s="13" t="s">
         <v>315</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>316</v>
       </c>
       <c r="P24" s="13" t="s">
         <v>25</v>
@@ -3174,7 +3174,7 @@
         <v>32</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="U24" s="1"/>
     </row>
@@ -3183,7 +3183,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>110</v>
@@ -3201,13 +3201,13 @@
         <v>113</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="K25" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="O25" s="13" t="s">
         <v>102</v>
@@ -3222,7 +3222,7 @@
         <v>203</v>
       </c>
       <c r="S25" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="U25" s="1"/>
     </row>
@@ -3231,7 +3231,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>114</v>
@@ -3249,13 +3249,13 @@
         <v>113</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K26" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="O26" s="13" t="s">
         <v>102</v>
@@ -3270,7 +3270,7 @@
         <v>203</v>
       </c>
       <c r="S26" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="U26" s="1"/>
     </row>
@@ -3279,7 +3279,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>117</v>
@@ -3297,16 +3297,16 @@
         <v>119</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K27" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="O27" s="13" t="s">
         <v>322</v>
-      </c>
-      <c r="O27" s="13" t="s">
-        <v>323</v>
       </c>
       <c r="P27" s="13" t="s">
         <v>25</v>
@@ -3327,7 +3327,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>120</v>
@@ -3366,7 +3366,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>123</v>
@@ -3384,16 +3384,16 @@
         <v>125</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K29" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="M29" s="9" t="s">
         <v>325</v>
-      </c>
-      <c r="M29" s="9" t="s">
-        <v>326</v>
       </c>
       <c r="P29" s="13" t="s">
         <v>25</v>
@@ -3405,7 +3405,7 @@
         <v>38</v>
       </c>
       <c r="S29" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="U29" s="1"/>
     </row>
@@ -3414,7 +3414,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>126</v>
@@ -3432,13 +3432,13 @@
         <v>128</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K30" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>329</v>
       </c>
       <c r="N30" s="13" t="s">
         <v>128</v>
@@ -3462,7 +3462,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>129</v>
@@ -3480,10 +3480,10 @@
         <v>131</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L31" s="13" t="s">
         <v>292</v>
@@ -3510,7 +3510,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>132</v>
@@ -3528,13 +3528,13 @@
         <v>134</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K32" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="L32" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>332</v>
       </c>
       <c r="N32" s="13" t="s">
         <v>134</v>
@@ -3558,7 +3558,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>135</v>
@@ -3576,13 +3576,13 @@
         <v>134</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K33" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>333</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>334</v>
       </c>
       <c r="N33" s="13" t="s">
         <v>134</v>
@@ -3606,7 +3606,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>137</v>
@@ -3645,7 +3645,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>139</v>
@@ -3663,13 +3663,13 @@
         <v>134</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K35" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>287</v>
@@ -3684,7 +3684,7 @@
         <v>32</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="U35" s="1"/>
     </row>
@@ -3693,7 +3693,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>141</v>
@@ -3711,13 +3711,13 @@
         <v>134</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K36" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="L36" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="N36" s="13" t="s">
         <v>134</v>
@@ -3741,7 +3741,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>143</v>
@@ -3759,13 +3759,13 @@
         <v>145</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K37" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="L37" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="N37" s="13" t="s">
         <v>146</v>
@@ -3789,7 +3789,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>147</v>
@@ -3801,7 +3801,7 @@
         <v>149</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>150</v>
@@ -3828,7 +3828,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>152</v>
@@ -3846,19 +3846,19 @@
         <v>155</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K39" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="L39" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="M39" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="M39" s="9" t="s">
+      <c r="O39" s="13" t="s">
         <v>343</v>
-      </c>
-      <c r="O39" s="13" t="s">
-        <v>344</v>
       </c>
       <c r="P39" s="13" t="s">
         <v>25</v>
@@ -3870,7 +3870,7 @@
         <v>38</v>
       </c>
       <c r="S39" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="U39" s="1"/>
     </row>
@@ -3879,7 +3879,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>156</v>
@@ -3891,7 +3891,7 @@
         <v>158</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>150</v>
@@ -3918,7 +3918,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>159</v>
@@ -3936,19 +3936,19 @@
         <v>155</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K41" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="L41" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>347</v>
-      </c>
       <c r="M41" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="O41" s="13" t="s">
         <v>343</v>
-      </c>
-      <c r="O41" s="13" t="s">
-        <v>344</v>
       </c>
       <c r="P41" s="13" t="s">
         <v>25</v>
@@ -3960,7 +3960,7 @@
         <v>38</v>
       </c>
       <c r="S41" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="U41" s="1"/>
     </row>
@@ -3969,7 +3969,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>162</v>
@@ -4008,7 +4008,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>165</v>
@@ -4026,13 +4026,13 @@
         <v>168</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K43" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>349</v>
       </c>
       <c r="N43" s="13" t="s">
         <v>168</v>
@@ -4056,7 +4056,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>169</v>
@@ -4074,19 +4074,19 @@
         <v>171</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K44" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="L44" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="M44" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="M44" s="9" t="s">
-        <v>352</v>
-      </c>
       <c r="O44" s="1" t="s">
-        <v>293</v>
+        <v>461</v>
       </c>
       <c r="P44" s="13" t="s">
         <v>25</v>
@@ -4098,7 +4098,7 @@
         <v>38</v>
       </c>
       <c r="S44" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="U44" s="1"/>
     </row>
@@ -4107,7 +4107,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>172</v>
@@ -4125,7 +4125,7 @@
         <v>175</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K45" s="13" t="s">
         <v>174</v>
@@ -4134,7 +4134,7 @@
         <v>173</v>
       </c>
       <c r="M45" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P45" s="1" t="s">
         <v>25</v>
@@ -4146,7 +4146,7 @@
         <v>38</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="U45" s="1"/>
     </row>
@@ -4155,7 +4155,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>176</v>
@@ -4175,7 +4175,7 @@
         <v>178</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K46" s="13" t="s">
         <v>174</v>
@@ -4184,7 +4184,7 @@
         <v>173</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="1" t="s">
@@ -4197,7 +4197,7 @@
         <v>38</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="U46" s="1"/>
     </row>
@@ -4206,7 +4206,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>179</v>
@@ -4224,19 +4224,19 @@
         <v>181</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K47" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="L47" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="N47" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="N47" s="13" t="s">
+      <c r="O47" s="13" t="s">
         <v>359</v>
-      </c>
-      <c r="O47" s="13" t="s">
-        <v>360</v>
       </c>
       <c r="P47" s="13" t="s">
         <v>25</v>
@@ -4248,7 +4248,7 @@
         <v>32</v>
       </c>
       <c r="S47" s="13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="U47" s="1"/>
     </row>
@@ -4257,7 +4257,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>182</v>
@@ -4275,16 +4275,16 @@
         <v>184</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K48" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="L48" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="M48" s="9" t="s">
         <v>362</v>
-      </c>
-      <c r="M48" s="9" t="s">
-        <v>363</v>
       </c>
       <c r="P48" s="13" t="s">
         <v>25</v>
@@ -4300,12 +4300,12 @@
       </c>
       <c r="U48" s="1"/>
     </row>
-    <row r="49" spans="1:21" ht="186" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>48</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>185</v>
@@ -4323,19 +4323,19 @@
         <v>188</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K49" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="L49" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="M49" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="M49" s="14" t="s">
+      <c r="O49" s="13" t="s">
         <v>366</v>
-      </c>
-      <c r="O49" s="13" t="s">
-        <v>367</v>
       </c>
       <c r="P49" s="13" t="s">
         <v>25</v>
@@ -4347,16 +4347,16 @@
         <v>203</v>
       </c>
       <c r="S49" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="U49" s="1"/>
     </row>
-    <row r="50" spans="1:21" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>49</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>189</v>
@@ -4374,19 +4374,19 @@
         <v>188</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K50" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="L50" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="M50" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="O50" s="13" t="s">
         <v>369</v>
-      </c>
-      <c r="M50" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="O50" s="13" t="s">
-        <v>370</v>
       </c>
       <c r="P50" s="13" t="s">
         <v>25</v>
@@ -4398,7 +4398,7 @@
         <v>203</v>
       </c>
       <c r="S50" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="U50" s="1"/>
     </row>
@@ -4407,7 +4407,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>192</v>
@@ -4425,16 +4425,16 @@
         <v>188</v>
       </c>
       <c r="J51" s="13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K51" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="L51" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="L51" s="1" t="s">
-        <v>372</v>
-      </c>
       <c r="M51" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="P51" s="13" t="s">
         <v>25</v>
@@ -4455,7 +4455,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>194</v>
@@ -4494,7 +4494,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>197</v>
@@ -4512,16 +4512,16 @@
         <v>188</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K53" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="L53" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="L53" s="1" t="s">
-        <v>374</v>
-      </c>
       <c r="M53" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="P53" s="13" t="s">
         <v>25</v>
@@ -4542,7 +4542,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>199</v>
@@ -4581,7 +4581,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>201</v>
@@ -4599,16 +4599,16 @@
         <v>188</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K55" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="L55" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="L55" s="1" t="s">
-        <v>376</v>
-      </c>
       <c r="M55" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="P55" s="13" t="s">
         <v>25</v>
@@ -4629,7 +4629,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>204</v>
@@ -4647,16 +4647,16 @@
         <v>188</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K56" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="L56" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="L56" s="1" t="s">
-        <v>378</v>
-      </c>
       <c r="M56" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="P56" s="13" t="s">
         <v>25</v>
@@ -4677,7 +4677,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>206</v>
@@ -4716,7 +4716,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>208</v>
@@ -4755,7 +4755,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>211</v>
@@ -4791,7 +4791,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>213</v>
@@ -4827,7 +4827,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C61" s="13" t="s">
         <v>215</v>
@@ -4863,7 +4863,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>217</v>
@@ -4899,7 +4899,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>219</v>
@@ -4935,7 +4935,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C64" s="13" t="s">
         <v>221</v>
@@ -4971,7 +4971,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>223</v>
@@ -5007,7 +5007,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>225</v>
@@ -5046,7 +5046,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C67" s="13" t="s">
         <v>228</v>
@@ -5064,16 +5064,16 @@
         <v>230</v>
       </c>
       <c r="J67" s="13" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K67" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="L67" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="L67" s="1" t="s">
+      <c r="O67" s="13" t="s">
         <v>380</v>
-      </c>
-      <c r="O67" s="13" t="s">
-        <v>381</v>
       </c>
       <c r="P67" s="13" t="s">
         <v>25</v>
@@ -5089,12 +5089,12 @@
       </c>
       <c r="U67" s="1"/>
     </row>
-    <row r="68" spans="1:21" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="256.5" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
         <v>67</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C68" s="13" t="s">
         <v>231</v>
@@ -5112,13 +5112,13 @@
         <v>233</v>
       </c>
       <c r="J68" s="13" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K68" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="L68" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="L68" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="P68" s="13" t="s">
         <v>25</v>
@@ -5130,7 +5130,7 @@
         <v>203</v>
       </c>
       <c r="S68" s="11" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="U68" s="1"/>
     </row>
@@ -5139,7 +5139,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C69" s="13" t="s">
         <v>234</v>
@@ -5157,16 +5157,16 @@
         <v>236</v>
       </c>
       <c r="J69" s="13" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K69" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="L69" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="L69" s="1" t="s">
+      <c r="M69" s="9" t="s">
         <v>383</v>
-      </c>
-      <c r="M69" s="9" t="s">
-        <v>384</v>
       </c>
       <c r="P69" s="13" t="s">
         <v>58</v>
@@ -5187,7 +5187,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C70" s="13" t="s">
         <v>237</v>
@@ -5205,16 +5205,16 @@
         <v>239</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K70" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="L70" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="L70" s="1" t="s">
+      <c r="M70" s="9" t="s">
         <v>386</v>
-      </c>
-      <c r="M70" s="9" t="s">
-        <v>387</v>
       </c>
       <c r="P70" s="13" t="s">
         <v>25</v>
@@ -5226,7 +5226,7 @@
         <v>38</v>
       </c>
       <c r="S70" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="U70" s="1"/>
     </row>
@@ -5235,7 +5235,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C71" s="13" t="s">
         <v>240</v>
@@ -5274,7 +5274,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C72" s="13" t="s">
         <v>242</v>
@@ -5313,7 +5313,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C73" s="13" t="s">
         <v>244</v>
@@ -5352,7 +5352,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>248</v>
@@ -5370,16 +5370,16 @@
         <v>251</v>
       </c>
       <c r="J74" s="13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K74" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="L74" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="L74" s="1" t="s">
-        <v>390</v>
-      </c>
       <c r="M74" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="P74" s="13" t="s">
         <v>25</v>
@@ -5391,7 +5391,7 @@
         <v>38</v>
       </c>
       <c r="S74" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="U74" s="1"/>
     </row>
@@ -5400,7 +5400,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>252</v>
@@ -5439,7 +5439,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>256</v>
@@ -5457,13 +5457,13 @@
         <v>230</v>
       </c>
       <c r="J76" s="13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K76" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="L76" s="1" t="s">
         <v>391</v>
-      </c>
-      <c r="L76" s="1" t="s">
-        <v>392</v>
       </c>
       <c r="P76" s="13" t="s">
         <v>25</v>
@@ -5479,12 +5479,12 @@
       </c>
       <c r="U76" s="1"/>
     </row>
-    <row r="77" spans="1:21" ht="327.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="114" x14ac:dyDescent="0.25">
       <c r="A77" s="13">
         <v>76</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>259</v>
@@ -5502,10 +5502,10 @@
         <v>262</v>
       </c>
       <c r="J77" s="13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K77" s="13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="P77" s="13" t="s">
         <v>25</v>
@@ -5517,7 +5517,7 @@
         <v>203</v>
       </c>
       <c r="S77" s="11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="U77" s="1"/>
     </row>
@@ -5526,7 +5526,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>263</v>
@@ -5565,7 +5565,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C79" s="13" t="s">
         <v>267</v>
@@ -5604,7 +5604,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>270</v>
@@ -5622,19 +5622,19 @@
         <v>188</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K80" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="L80" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="L80" s="1" t="s">
+      <c r="M80" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="M80" s="9" t="s">
+      <c r="O80" s="13" t="s">
         <v>395</v>
-      </c>
-      <c r="O80" s="13" t="s">
-        <v>396</v>
       </c>
       <c r="P80" s="13" t="s">
         <v>25</v>
@@ -5655,7 +5655,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C81" s="13" t="s">
         <v>273</v>
@@ -5694,7 +5694,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>276</v>
@@ -5733,7 +5733,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>279</v>
@@ -5769,7 +5769,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>282</v>

</xml_diff>

<commit_message>
correcting sport participation recoding
</commit_message>
<xml_diff>
--- a/data_processing_elements-NHS.xlsx
+++ b/data_processing_elements-NHS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E66CE4-4D35-4817-B88B-2B43258B617B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6109F512-E5BF-4861-A2C5-E556E9EC03C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -967,9 +967,6 @@
     <t>items</t>
   </si>
   <si>
-    <t>recode(1=0; 2=1; 3=1; 4=1; 5=1; ELSE=NA)</t>
-  </si>
-  <si>
     <t>Friedewald equation was used https://lipidworld.biomedcentral.com/articles/10.1186/1476-511X-9-27</t>
   </si>
   <si>
@@ -1616,6 +1613,9 @@
   </si>
   <si>
     <t>4 times a week or more is considered as dayly/almost daily</t>
+  </si>
+  <si>
+    <t>recode(1=1; 2=1; 3=1; 4=1; 5=0; ELSE=NA)</t>
   </si>
 </sst>
 </file>
@@ -1710,7 +1710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1752,9 +1752,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1776,7 +1779,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2095,13 +2098,13 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="13" customWidth="1"/>
@@ -2196,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>21</v>
@@ -2211,10 +2214,10 @@
         <v>24</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="P2" s="13" t="s">
         <v>25</v>
@@ -2223,13 +2226,13 @@
         <v>26</v>
       </c>
       <c r="R2" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="S2" s="13" t="s">
         <v>399</v>
       </c>
-      <c r="S2" s="13" t="s">
-        <v>400</v>
-      </c>
       <c r="T2" s="16" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="U2" s="1"/>
     </row>
@@ -2238,7 +2241,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>27</v>
@@ -2256,16 +2259,16 @@
         <v>31</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K3" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="N3" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="P3" s="13" t="s">
         <v>25</v>
@@ -2277,7 +2280,7 @@
         <v>32</v>
       </c>
       <c r="S3" s="13" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
@@ -2287,7 +2290,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>33</v>
@@ -2326,7 +2329,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>39</v>
@@ -2344,13 +2347,13 @@
         <v>42</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P5" s="13" t="s">
         <v>25</v>
@@ -2362,7 +2365,7 @@
         <v>32</v>
       </c>
       <c r="S5" s="13" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="U5" s="1"/>
     </row>
@@ -2371,7 +2374,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>44</v>
@@ -2389,16 +2392,16 @@
         <v>47</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="M6" s="9" t="s">
         <v>299</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>300</v>
       </c>
       <c r="P6" s="13" t="s">
         <v>25</v>
@@ -2410,7 +2413,7 @@
         <v>38</v>
       </c>
       <c r="S6" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -2420,7 +2423,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>49</v>
@@ -2459,7 +2462,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>54</v>
@@ -2477,13 +2480,13 @@
         <v>57</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K8" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="P8" s="13" t="s">
         <v>25</v>
@@ -2504,7 +2507,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>60</v>
@@ -2522,16 +2525,16 @@
         <v>63</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K9" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="O9" s="13" t="s">
         <v>304</v>
-      </c>
-      <c r="O9" s="13" t="s">
-        <v>305</v>
       </c>
       <c r="P9" s="13" t="s">
         <v>25</v>
@@ -2543,7 +2546,7 @@
         <v>38</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="U9" s="1"/>
     </row>
@@ -2552,7 +2555,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>64</v>
@@ -2589,7 +2592,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>68</v>
@@ -2604,16 +2607,16 @@
         <v>24</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="9" t="s">
         <v>307</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>308</v>
       </c>
       <c r="P11" s="13" t="s">
         <v>25</v>
@@ -2625,7 +2628,7 @@
         <v>203</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="U11" s="1"/>
     </row>
@@ -2634,7 +2637,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>71</v>
@@ -2673,7 +2676,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>75</v>
@@ -2691,16 +2694,16 @@
         <v>78</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P13" s="13" t="s">
         <v>25</v>
@@ -2712,7 +2715,7 @@
         <v>38</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U13" s="1"/>
     </row>
@@ -2721,7 +2724,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>79</v>
@@ -2760,7 +2763,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>83</v>
@@ -2778,13 +2781,13 @@
         <v>85</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P15" s="13" t="s">
         <v>25</v>
@@ -2799,7 +2802,7 @@
         <v>43</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="U15" s="1"/>
     </row>
@@ -2808,7 +2811,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>86</v>
@@ -2826,10 +2829,10 @@
         <v>88</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="P16" s="13" t="s">
         <v>25</v>
@@ -2850,7 +2853,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>89</v>
@@ -2868,7 +2871,7 @@
         <v>91</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="P17" s="13" t="s">
         <v>25</v>
@@ -2880,7 +2883,7 @@
         <v>32</v>
       </c>
       <c r="S17" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
@@ -2890,7 +2893,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>92</v>
@@ -2908,10 +2911,10 @@
         <v>94</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P18" s="13" t="s">
         <v>25</v>
@@ -2932,7 +2935,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>95</v>
@@ -2950,7 +2953,7 @@
         <v>91</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="P19" s="13" t="s">
         <v>25</v>
@@ -2962,7 +2965,7 @@
         <v>32</v>
       </c>
       <c r="S19" s="13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -2972,7 +2975,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>97</v>
@@ -2990,10 +2993,10 @@
         <v>99</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P20" s="13" t="s">
         <v>25</v>
@@ -3014,7 +3017,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>100</v>
@@ -3032,10 +3035,10 @@
         <v>88</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P21" s="13" t="s">
         <v>25</v>
@@ -3056,7 +3059,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>103</v>
@@ -3074,7 +3077,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="P22" s="13" t="s">
         <v>25</v>
@@ -3086,7 +3089,7 @@
         <v>32</v>
       </c>
       <c r="S22" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -3096,7 +3099,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>105</v>
@@ -3114,13 +3117,13 @@
         <v>107</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K23" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="L23" s="13" t="s">
         <v>314</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>315</v>
       </c>
       <c r="P23" s="13" t="s">
         <v>25</v>
@@ -3141,7 +3144,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>108</v>
@@ -3156,13 +3159,13 @@
         <v>24</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K24" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="L24" s="13" t="s">
         <v>314</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>315</v>
       </c>
       <c r="P24" s="13" t="s">
         <v>25</v>
@@ -3174,7 +3177,7 @@
         <v>32</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="U24" s="1"/>
     </row>
@@ -3183,7 +3186,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>110</v>
@@ -3201,13 +3204,13 @@
         <v>113</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K25" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>317</v>
       </c>
       <c r="O25" s="13" t="s">
         <v>102</v>
@@ -3222,7 +3225,7 @@
         <v>203</v>
       </c>
       <c r="S25" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="U25" s="1"/>
     </row>
@@ -3231,7 +3234,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>114</v>
@@ -3249,13 +3252,13 @@
         <v>113</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="K26" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>319</v>
       </c>
       <c r="O26" s="13" t="s">
         <v>102</v>
@@ -3270,7 +3273,7 @@
         <v>203</v>
       </c>
       <c r="S26" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="U26" s="1"/>
     </row>
@@ -3279,7 +3282,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>117</v>
@@ -3297,16 +3300,16 @@
         <v>119</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K27" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="O27" s="13" t="s">
         <v>321</v>
-      </c>
-      <c r="O27" s="13" t="s">
-        <v>322</v>
       </c>
       <c r="P27" s="13" t="s">
         <v>25</v>
@@ -3327,7 +3330,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>120</v>
@@ -3366,7 +3369,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>123</v>
@@ -3384,16 +3387,16 @@
         <v>125</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K29" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="M29" s="9" t="s">
         <v>324</v>
-      </c>
-      <c r="M29" s="9" t="s">
-        <v>325</v>
       </c>
       <c r="P29" s="13" t="s">
         <v>25</v>
@@ -3405,7 +3408,7 @@
         <v>38</v>
       </c>
       <c r="S29" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="U29" s="1"/>
     </row>
@@ -3414,7 +3417,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>126</v>
@@ -3432,13 +3435,13 @@
         <v>128</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K30" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>328</v>
       </c>
       <c r="N30" s="13" t="s">
         <v>128</v>
@@ -3462,7 +3465,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>129</v>
@@ -3480,13 +3483,13 @@
         <v>131</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>131</v>
@@ -3510,7 +3513,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>132</v>
@@ -3528,13 +3531,13 @@
         <v>134</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K32" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="L32" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>331</v>
       </c>
       <c r="N32" s="13" t="s">
         <v>134</v>
@@ -3558,7 +3561,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>135</v>
@@ -3576,13 +3579,13 @@
         <v>134</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K33" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="N33" s="13" t="s">
         <v>134</v>
@@ -3606,7 +3609,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>137</v>
@@ -3645,7 +3648,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>139</v>
@@ -3663,16 +3666,16 @@
         <v>134</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K35" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="O35" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P35" s="13" t="s">
         <v>25</v>
@@ -3684,7 +3687,7 @@
         <v>32</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="U35" s="1"/>
     </row>
@@ -3693,7 +3696,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>141</v>
@@ -3711,13 +3714,13 @@
         <v>134</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K36" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="L36" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>337</v>
       </c>
       <c r="N36" s="13" t="s">
         <v>134</v>
@@ -3741,7 +3744,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>143</v>
@@ -3759,13 +3762,13 @@
         <v>145</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K37" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="L37" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>339</v>
       </c>
       <c r="N37" s="13" t="s">
         <v>146</v>
@@ -3789,7 +3792,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>147</v>
@@ -3828,7 +3831,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>152</v>
@@ -3846,19 +3849,19 @@
         <v>155</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K39" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="L39" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="M39" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="M39" s="9" t="s">
+      <c r="O39" s="13" t="s">
         <v>342</v>
-      </c>
-      <c r="O39" s="13" t="s">
-        <v>343</v>
       </c>
       <c r="P39" s="13" t="s">
         <v>25</v>
@@ -3870,7 +3873,7 @@
         <v>38</v>
       </c>
       <c r="S39" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="U39" s="1"/>
     </row>
@@ -3879,7 +3882,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>156</v>
@@ -3918,7 +3921,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>159</v>
@@ -3936,19 +3939,19 @@
         <v>155</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K41" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="L41" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>346</v>
-      </c>
       <c r="M41" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="O41" s="13" t="s">
         <v>342</v>
-      </c>
-      <c r="O41" s="13" t="s">
-        <v>343</v>
       </c>
       <c r="P41" s="13" t="s">
         <v>25</v>
@@ -3960,7 +3963,7 @@
         <v>38</v>
       </c>
       <c r="S41" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="U41" s="1"/>
     </row>
@@ -3969,7 +3972,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>162</v>
@@ -4008,7 +4011,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>165</v>
@@ -4026,13 +4029,13 @@
         <v>168</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K43" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>348</v>
       </c>
       <c r="N43" s="13" t="s">
         <v>168</v>
@@ -4056,7 +4059,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>169</v>
@@ -4074,19 +4077,19 @@
         <v>171</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K44" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="L44" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="M44" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="M44" s="9" t="s">
-        <v>351</v>
-      </c>
       <c r="O44" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="P44" s="13" t="s">
         <v>25</v>
@@ -4098,7 +4101,7 @@
         <v>38</v>
       </c>
       <c r="S44" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="U44" s="1"/>
     </row>
@@ -4107,7 +4110,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>172</v>
@@ -4125,7 +4128,7 @@
         <v>175</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K45" s="13" t="s">
         <v>174</v>
@@ -4134,7 +4137,7 @@
         <v>173</v>
       </c>
       <c r="M45" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P45" s="1" t="s">
         <v>25</v>
@@ -4146,7 +4149,7 @@
         <v>38</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="U45" s="1"/>
     </row>
@@ -4155,7 +4158,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>176</v>
@@ -4175,7 +4178,7 @@
         <v>178</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K46" s="13" t="s">
         <v>174</v>
@@ -4184,7 +4187,7 @@
         <v>173</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="1" t="s">
@@ -4197,7 +4200,7 @@
         <v>38</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="U46" s="1"/>
     </row>
@@ -4206,7 +4209,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>179</v>
@@ -4224,19 +4227,19 @@
         <v>181</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K47" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="L47" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="N47" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="N47" s="13" t="s">
+      <c r="O47" s="13" t="s">
         <v>358</v>
-      </c>
-      <c r="O47" s="13" t="s">
-        <v>359</v>
       </c>
       <c r="P47" s="13" t="s">
         <v>25</v>
@@ -4248,7 +4251,7 @@
         <v>32</v>
       </c>
       <c r="S47" s="13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="U47" s="1"/>
     </row>
@@ -4257,7 +4260,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>182</v>
@@ -4275,16 +4278,16 @@
         <v>184</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K48" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="L48" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="M48" s="9" t="s">
         <v>361</v>
-      </c>
-      <c r="M48" s="9" t="s">
-        <v>362</v>
       </c>
       <c r="P48" s="13" t="s">
         <v>25</v>
@@ -4305,7 +4308,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>185</v>
@@ -4323,19 +4326,19 @@
         <v>188</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K49" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="L49" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="M49" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="M49" s="14" t="s">
+      <c r="O49" s="13" t="s">
         <v>365</v>
-      </c>
-      <c r="O49" s="13" t="s">
-        <v>366</v>
       </c>
       <c r="P49" s="13" t="s">
         <v>25</v>
@@ -4347,7 +4350,7 @@
         <v>203</v>
       </c>
       <c r="S49" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="U49" s="1"/>
     </row>
@@ -4356,7 +4359,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>189</v>
@@ -4374,19 +4377,19 @@
         <v>188</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K50" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="L50" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="M50" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="O50" s="13" t="s">
         <v>368</v>
-      </c>
-      <c r="M50" s="14" t="s">
-        <v>365</v>
-      </c>
-      <c r="O50" s="13" t="s">
-        <v>369</v>
       </c>
       <c r="P50" s="13" t="s">
         <v>25</v>
@@ -4398,7 +4401,7 @@
         <v>203</v>
       </c>
       <c r="S50" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="U50" s="1"/>
     </row>
@@ -4407,7 +4410,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>192</v>
@@ -4425,16 +4428,16 @@
         <v>188</v>
       </c>
       <c r="J51" s="13" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K51" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="L51" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="L51" s="1" t="s">
-        <v>371</v>
-      </c>
       <c r="M51" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P51" s="13" t="s">
         <v>25</v>
@@ -4455,7 +4458,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>194</v>
@@ -4494,7 +4497,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>197</v>
@@ -4512,16 +4515,16 @@
         <v>188</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K53" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="L53" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="L53" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="M53" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P53" s="13" t="s">
         <v>25</v>
@@ -4542,7 +4545,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>199</v>
@@ -4581,7 +4584,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>201</v>
@@ -4599,16 +4602,16 @@
         <v>188</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K55" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="L55" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="L55" s="1" t="s">
-        <v>375</v>
-      </c>
       <c r="M55" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P55" s="13" t="s">
         <v>25</v>
@@ -4629,7 +4632,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>204</v>
@@ -4647,16 +4650,16 @@
         <v>188</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K56" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="L56" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="L56" s="1" t="s">
-        <v>377</v>
-      </c>
       <c r="M56" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P56" s="13" t="s">
         <v>25</v>
@@ -4677,7 +4680,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>206</v>
@@ -4716,7 +4719,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>208</v>
@@ -4755,7 +4758,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>211</v>
@@ -4791,7 +4794,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>213</v>
@@ -4827,7 +4830,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C61" s="13" t="s">
         <v>215</v>
@@ -4863,7 +4866,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>217</v>
@@ -4899,7 +4902,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>219</v>
@@ -4935,7 +4938,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C64" s="13" t="s">
         <v>221</v>
@@ -4971,7 +4974,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>223</v>
@@ -5007,7 +5010,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>225</v>
@@ -5046,7 +5049,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C67" s="13" t="s">
         <v>228</v>
@@ -5064,16 +5067,16 @@
         <v>230</v>
       </c>
       <c r="J67" s="13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K67" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="L67" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="L67" s="1" t="s">
+      <c r="O67" s="13" t="s">
         <v>379</v>
-      </c>
-      <c r="O67" s="13" t="s">
-        <v>380</v>
       </c>
       <c r="P67" s="13" t="s">
         <v>25</v>
@@ -5094,7 +5097,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C68" s="13" t="s">
         <v>231</v>
@@ -5112,13 +5115,13 @@
         <v>233</v>
       </c>
       <c r="J68" s="13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K68" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="L68" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="L68" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="P68" s="13" t="s">
         <v>25</v>
@@ -5130,7 +5133,7 @@
         <v>203</v>
       </c>
       <c r="S68" s="11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="U68" s="1"/>
     </row>
@@ -5139,7 +5142,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C69" s="13" t="s">
         <v>234</v>
@@ -5157,16 +5160,16 @@
         <v>236</v>
       </c>
       <c r="J69" s="13" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K69" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="L69" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="L69" s="1" t="s">
+      <c r="M69" s="9" t="s">
         <v>382</v>
-      </c>
-      <c r="M69" s="9" t="s">
-        <v>383</v>
       </c>
       <c r="P69" s="13" t="s">
         <v>58</v>
@@ -5187,7 +5190,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C70" s="13" t="s">
         <v>237</v>
@@ -5205,16 +5208,16 @@
         <v>239</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K70" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="L70" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="L70" s="1" t="s">
+      <c r="M70" s="9" t="s">
         <v>385</v>
-      </c>
-      <c r="M70" s="9" t="s">
-        <v>386</v>
       </c>
       <c r="P70" s="13" t="s">
         <v>25</v>
@@ -5226,7 +5229,7 @@
         <v>38</v>
       </c>
       <c r="S70" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="U70" s="1"/>
     </row>
@@ -5235,7 +5238,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C71" s="13" t="s">
         <v>240</v>
@@ -5274,7 +5277,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C72" s="13" t="s">
         <v>242</v>
@@ -5313,7 +5316,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C73" s="13" t="s">
         <v>244</v>
@@ -5352,7 +5355,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>248</v>
@@ -5370,16 +5373,16 @@
         <v>251</v>
       </c>
       <c r="J74" s="13" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K74" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="L74" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="L74" s="1" t="s">
-        <v>389</v>
-      </c>
       <c r="M74" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="P74" s="13" t="s">
         <v>25</v>
@@ -5391,7 +5394,7 @@
         <v>38</v>
       </c>
       <c r="S74" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="U74" s="1"/>
     </row>
@@ -5400,7 +5403,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>252</v>
@@ -5439,7 +5442,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>256</v>
@@ -5457,13 +5460,13 @@
         <v>230</v>
       </c>
       <c r="J76" s="13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K76" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="L76" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="L76" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="P76" s="13" t="s">
         <v>25</v>
@@ -5484,7 +5487,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>259</v>
@@ -5502,10 +5505,10 @@
         <v>262</v>
       </c>
       <c r="J77" s="13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K77" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="P77" s="13" t="s">
         <v>25</v>
@@ -5517,7 +5520,7 @@
         <v>203</v>
       </c>
       <c r="S77" s="11" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="U77" s="1"/>
     </row>
@@ -5526,7 +5529,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>263</v>
@@ -5565,7 +5568,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C79" s="13" t="s">
         <v>267</v>
@@ -5599,12 +5602,12 @@
       </c>
       <c r="U79" s="1"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A80" s="13">
         <v>79</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>270</v>
@@ -5622,19 +5625,19 @@
         <v>188</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K80" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="L80" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="L80" s="1" t="s">
+      <c r="M80" s="17" t="s">
         <v>393</v>
       </c>
-      <c r="M80" s="9" t="s">
+      <c r="O80" s="13" t="s">
         <v>394</v>
-      </c>
-      <c r="O80" s="13" t="s">
-        <v>395</v>
       </c>
       <c r="P80" s="13" t="s">
         <v>25</v>
@@ -5646,7 +5649,7 @@
         <v>38</v>
       </c>
       <c r="S80" s="13" t="s">
-        <v>286</v>
+        <v>461</v>
       </c>
       <c r="U80" s="1"/>
     </row>
@@ -5655,7 +5658,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C81" s="13" t="s">
         <v>273</v>
@@ -5694,7 +5697,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>276</v>
@@ -5733,7 +5736,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>279</v>
@@ -5769,7 +5772,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>282</v>

</xml_diff>